<commit_message>
Video: add api for video tag
</commit_message>
<xml_diff>
--- a/public/sample/video_batch_sample.xlsx
+++ b/public/sample/video_batch_sample.xlsx
@@ -8,15 +8,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="+c3hqAOZ5e7W+cOTSIOnR5IciIiyz6unUwVoDkQxTVA="/>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj+w0C4o58NgrpAFbzV0jJoYAB/NQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="99">
   <si>
     <t>title</t>
   </si>
@@ -27,7 +27,7 @@
     <t>author</t>
   </si>
   <si>
-    <t>category</t>
+    <t>tag_list</t>
   </si>
   <si>
     <t>ភាពពេញវ័យ</t>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>RHAC</t>
+  </si>
+  <si>
+    <t>ភាពពេញវ័យ,សុខភាពបន្តពូជ</t>
   </si>
   <si>
     <t>ការរំលូតដោយសុវត្ថិភាព</t>
@@ -316,7 +319,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -335,6 +338,11 @@
     <font>
       <u/>
       <color rgb="FF0000FF"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -357,19 +365,22 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
@@ -593,17 +604,16 @@
     <col customWidth="1" min="1" max="1" width="44.13"/>
     <col customWidth="1" min="2" max="2" width="44.5"/>
     <col customWidth="1" min="3" max="3" width="28.25"/>
-    <col customWidth="1" min="4" max="5" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -620,13 +630,16 @@
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -634,10 +647,10 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -645,10 +658,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>6</v>
@@ -656,10 +669,10 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>6</v>
@@ -667,10 +680,10 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>6</v>
@@ -678,43 +691,43 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -722,10 +735,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>6</v>
@@ -733,10 +746,10 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>
@@ -744,10 +757,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>6</v>
@@ -755,10 +768,10 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>6</v>
@@ -766,43 +779,43 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -810,10 +823,10 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
@@ -821,10 +834,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>6</v>
@@ -832,21 +845,21 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>6</v>
@@ -854,10 +867,10 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>6</v>
@@ -865,10 +878,10 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>6</v>
@@ -876,10 +889,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>6</v>
@@ -887,10 +900,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>6</v>
@@ -898,779 +911,779 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="B44" s="5"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="B45" s="5"/>
+      <c r="B45" s="6"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="B46" s="5"/>
+      <c r="B46" s="6"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="B47" s="5"/>
+      <c r="B47" s="6"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="B48" s="5"/>
+      <c r="B48" s="6"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="B49" s="5"/>
+      <c r="B49" s="6"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="B50" s="5"/>
+      <c r="B50" s="6"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="B51" s="5"/>
+      <c r="B51" s="6"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="B52" s="5"/>
+      <c r="B52" s="6"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="B53" s="5"/>
+      <c r="B53" s="6"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="B54" s="5"/>
+      <c r="B54" s="6"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="B55" s="5"/>
+      <c r="B55" s="6"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="B56" s="5"/>
+      <c r="B56" s="6"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="B57" s="5"/>
+      <c r="B57" s="6"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="B58" s="5"/>
+      <c r="B58" s="6"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="B59" s="5"/>
+      <c r="B59" s="6"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="B60" s="5"/>
+      <c r="B60" s="6"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="5"/>
+      <c r="B61" s="6"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="B62" s="5"/>
+      <c r="B62" s="6"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="5"/>
+      <c r="B63" s="6"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="5"/>
+      <c r="B64" s="6"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="B65" s="5"/>
+      <c r="B65" s="6"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="B66" s="5"/>
+      <c r="B66" s="6"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="B67" s="5"/>
+      <c r="B67" s="6"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="B68" s="5"/>
+      <c r="B68" s="6"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="B69" s="5"/>
+      <c r="B69" s="6"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="B70" s="5"/>
+      <c r="B70" s="6"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="B71" s="5"/>
+      <c r="B71" s="6"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="B72" s="5"/>
+      <c r="B72" s="6"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="B73" s="5"/>
+      <c r="B73" s="6"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="B74" s="5"/>
+      <c r="B74" s="6"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="B75" s="5"/>
+      <c r="B75" s="6"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="B76" s="5"/>
+      <c r="B76" s="6"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="B77" s="5"/>
+      <c r="B77" s="6"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="B78" s="5"/>
+      <c r="B78" s="6"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="B79" s="5"/>
+      <c r="B79" s="6"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="B80" s="5"/>
+      <c r="B80" s="6"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="B81" s="5"/>
+      <c r="B81" s="6"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="B82" s="5"/>
+      <c r="B82" s="6"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="B83" s="5"/>
+      <c r="B83" s="6"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="B84" s="5"/>
+      <c r="B84" s="6"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="B85" s="5"/>
+      <c r="B85" s="6"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="B86" s="5"/>
+      <c r="B86" s="6"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="B87" s="5"/>
+      <c r="B87" s="6"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="B88" s="5"/>
+      <c r="B88" s="6"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="B89" s="5"/>
+      <c r="B89" s="6"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="B90" s="5"/>
+      <c r="B90" s="6"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="B91" s="5"/>
+      <c r="B91" s="6"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="B92" s="5"/>
+      <c r="B92" s="6"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="B93" s="5"/>
+      <c r="B93" s="6"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="B94" s="5"/>
+      <c r="B94" s="6"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="B95" s="5"/>
+      <c r="B95" s="6"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="B96" s="5"/>
+      <c r="B96" s="6"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="B97" s="5"/>
+      <c r="B97" s="6"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="B98" s="5"/>
+      <c r="B98" s="6"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="B99" s="5"/>
+      <c r="B99" s="6"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="B100" s="5"/>
+      <c r="B100" s="6"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="B101" s="5"/>
+      <c r="B101" s="6"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="B102" s="5"/>
+      <c r="B102" s="6"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="B103" s="5"/>
+      <c r="B103" s="6"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="B104" s="5"/>
+      <c r="B104" s="6"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="B105" s="5"/>
+      <c r="B105" s="6"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="B106" s="5"/>
+      <c r="B106" s="6"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="B107" s="5"/>
+      <c r="B107" s="6"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="B108" s="5"/>
+      <c r="B108" s="6"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="B109" s="5"/>
+      <c r="B109" s="6"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="B110" s="5"/>
+      <c r="B110" s="6"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="B111" s="5"/>
+      <c r="B111" s="6"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="B112" s="5"/>
+      <c r="B112" s="6"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="B113" s="5"/>
+      <c r="B113" s="6"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="B114" s="5"/>
+      <c r="B114" s="6"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="B115" s="5"/>
+      <c r="B115" s="6"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="B116" s="5"/>
+      <c r="B116" s="6"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="B117" s="5"/>
+      <c r="B117" s="6"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="B118" s="5"/>
+      <c r="B118" s="6"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="B119" s="5"/>
+      <c r="B119" s="6"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="B120" s="5"/>
+      <c r="B120" s="6"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="B121" s="5"/>
+      <c r="B121" s="6"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="B122" s="5"/>
+      <c r="B122" s="6"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="B123" s="5"/>
+      <c r="B123" s="6"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="B124" s="5"/>
+      <c r="B124" s="6"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="B125" s="5"/>
+      <c r="B125" s="6"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="B126" s="5"/>
+      <c r="B126" s="6"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="B127" s="5"/>
+      <c r="B127" s="6"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="B128" s="5"/>
+      <c r="B128" s="6"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="B129" s="5"/>
+      <c r="B129" s="6"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="B130" s="5"/>
+      <c r="B130" s="6"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="B131" s="5"/>
+      <c r="B131" s="6"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="B132" s="5"/>
+      <c r="B132" s="6"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="B133" s="5"/>
+      <c r="B133" s="6"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="B134" s="5"/>
+      <c r="B134" s="6"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="B135" s="5"/>
+      <c r="B135" s="6"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="B136" s="5"/>
+      <c r="B136" s="6"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="B137" s="5"/>
+      <c r="B137" s="6"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="B138" s="5"/>
+      <c r="B138" s="6"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="B139" s="5"/>
+      <c r="B139" s="6"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="B140" s="5"/>
+      <c r="B140" s="6"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="B141" s="5"/>
+      <c r="B141" s="6"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="B142" s="5"/>
+      <c r="B142" s="6"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="B143" s="5"/>
+      <c r="B143" s="6"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="B144" s="5"/>
+      <c r="B144" s="6"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="B145" s="5"/>
+      <c r="B145" s="6"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="B146" s="5"/>
+      <c r="B146" s="6"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="B147" s="5"/>
+      <c r="B147" s="6"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="B148" s="5"/>
+      <c r="B148" s="6"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="B149" s="5"/>
+      <c r="B149" s="6"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="B150" s="5"/>
+      <c r="B150" s="6"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="B151" s="5"/>
+      <c r="B151" s="6"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="B152" s="5"/>
+      <c r="B152" s="6"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="B153" s="5"/>
+      <c r="B153" s="6"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="B154" s="5"/>
+      <c r="B154" s="6"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="B155" s="5"/>
+      <c r="B155" s="6"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="B156" s="5"/>
+      <c r="B156" s="6"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="B157" s="5"/>
+      <c r="B157" s="6"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="B158" s="5"/>
+      <c r="B158" s="6"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="B159" s="5"/>
+      <c r="B159" s="6"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="B160" s="5"/>
+      <c r="B160" s="6"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="B161" s="5"/>
+      <c r="B161" s="6"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="B162" s="5"/>
+      <c r="B162" s="6"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="B163" s="5"/>
+      <c r="B163" s="6"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="B164" s="5"/>
+      <c r="B164" s="6"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="B165" s="5"/>
+      <c r="B165" s="6"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="B166" s="5"/>
+      <c r="B166" s="6"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="B167" s="5"/>
+      <c r="B167" s="6"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="B168" s="5"/>
+      <c r="B168" s="6"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="B169" s="5"/>
+      <c r="B169" s="6"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="B170" s="5"/>
+      <c r="B170" s="6"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="B171" s="5"/>
+      <c r="B171" s="6"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="B172" s="5"/>
+      <c r="B172" s="6"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="B173" s="5"/>
+      <c r="B173" s="6"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="B174" s="5"/>
+      <c r="B174" s="6"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="B175" s="5"/>
+      <c r="B175" s="6"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="B176" s="5"/>
+      <c r="B176" s="6"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="B177" s="5"/>
+      <c r="B177" s="6"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="B178" s="5"/>
+      <c r="B178" s="6"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="B179" s="5"/>
+      <c r="B179" s="6"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="B180" s="5"/>
+      <c r="B180" s="6"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="B181" s="5"/>
+      <c r="B181" s="6"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="B182" s="5"/>
+      <c r="B182" s="6"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="B183" s="5"/>
+      <c r="B183" s="6"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="B184" s="5"/>
+      <c r="B184" s="6"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="B185" s="5"/>
+      <c r="B185" s="6"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="B186" s="5"/>
+      <c r="B186" s="6"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="B187" s="5"/>
+      <c r="B187" s="6"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="B188" s="5"/>
+      <c r="B188" s="6"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="B189" s="5"/>
+      <c r="B189" s="6"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="B190" s="5"/>
+      <c r="B190" s="6"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="B191" s="5"/>
+      <c r="B191" s="6"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="B192" s="5"/>
+      <c r="B192" s="6"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="B193" s="5"/>
+      <c r="B193" s="6"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="B194" s="5"/>
+      <c r="B194" s="6"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="B195" s="5"/>
+      <c r="B195" s="6"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="B196" s="5"/>
+      <c r="B196" s="6"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="B197" s="5"/>
+      <c r="B197" s="6"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="B198" s="5"/>
+      <c r="B198" s="6"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="B199" s="5"/>
+      <c r="B199" s="6"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="B200" s="5"/>
+      <c r="B200" s="6"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="B201" s="5"/>
+      <c r="B201" s="6"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="B202" s="5"/>
+      <c r="B202" s="6"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="B203" s="5"/>
+      <c r="B203" s="6"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="B204" s="5"/>
+      <c r="B204" s="6"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="B205" s="5"/>
+      <c r="B205" s="6"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="B206" s="5"/>
+      <c r="B206" s="6"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="B207" s="5"/>
+      <c r="B207" s="6"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="B208" s="5"/>
+      <c r="B208" s="6"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="B209" s="5"/>
+      <c r="B209" s="6"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="B210" s="5"/>
+      <c r="B210" s="6"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="B211" s="5"/>
+      <c r="B211" s="6"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="B212" s="5"/>
+      <c r="B212" s="6"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="B213" s="5"/>
+      <c r="B213" s="6"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="B214" s="5"/>
+      <c r="B214" s="6"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="B215" s="5"/>
+      <c r="B215" s="6"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="B216" s="5"/>
+      <c r="B216" s="6"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="B217" s="5"/>
+      <c r="B217" s="6"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="B218" s="5"/>
+      <c r="B218" s="6"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="B219" s="5"/>
+      <c r="B219" s="6"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="B220" s="5"/>
+      <c r="B220" s="6"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="B221" s="5"/>
+      <c r="B221" s="6"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="B222" s="5"/>
+      <c r="B222" s="6"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="B223" s="5"/>
+      <c r="B223" s="6"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="B224" s="5"/>
+      <c r="B224" s="6"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="B225" s="5"/>
+      <c r="B225" s="6"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="B226" s="5"/>
+      <c r="B226" s="6"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="B227" s="5"/>
+      <c r="B227" s="6"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="B228" s="5"/>
+      <c r="B228" s="6"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="B229" s="5"/>
+      <c r="B229" s="6"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="B230" s="5"/>
+      <c r="B230" s="6"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="B231" s="5"/>
+      <c r="B231" s="6"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="B232" s="5"/>
+      <c r="B232" s="6"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="B233" s="5"/>
+      <c r="B233" s="6"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="B234" s="5"/>
+      <c r="B234" s="6"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="B235" s="5"/>
+      <c r="B235" s="6"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="B236" s="5"/>
+      <c r="B236" s="6"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="B237" s="5"/>
+      <c r="B237" s="6"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="B238" s="5"/>
+      <c r="B238" s="6"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="B239" s="5"/>
+      <c r="B239" s="6"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="B240" s="5"/>
+      <c r="B240" s="6"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="B241" s="5"/>
+      <c r="B241" s="6"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="B242" s="5"/>
+      <c r="B242" s="6"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="B243" s="5"/>
+      <c r="B243" s="6"/>
     </row>
     <row r="244" ht="15.75" customHeight="1"/>
     <row r="245" ht="15.75" customHeight="1"/>

</xml_diff>